<commit_message>
Add new NCC with feature
</commit_message>
<xml_diff>
--- a/New Dataset HistogramxFeature/Experiment result NCC with feature/Sit Long/Accuracy round 1/NCC with feature Accuracy Training sit_long .xlsx
+++ b/New Dataset HistogramxFeature/Experiment result NCC with feature/Sit Long/Accuracy round 1/NCC with feature Accuracy Training sit_long .xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20350"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20351"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Matlab\Mobile Authentication\New Dataset HistogramxFeature\Experiment result NCC with feature\Sit Long\Accuracy round 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A184502-3BF0-4C2F-8714-4A3A5390E39A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3855C117-D77B-4DB2-9C94-E66BCA68F8F0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16170" windowHeight="8190" firstSheet="2" activeTab="3" xr2:uid="{394EE492-C35C-4FE7-A850-7F2E69943D7D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="10215" activeTab="3" xr2:uid="{8E561005-FB62-4DB9-BD4A-EDE3BA663698}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -373,7 +373,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD4691F1-A5AB-4980-9A88-71212A0F4EAD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29E23B06-91DD-4452-8478-B40D44D92166}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -385,7 +385,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A810A0A7-6629-40C6-A01A-DAF94E6EBE90}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4E36216-5001-4C17-B840-31AA8D07C791}">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -396,30 +396,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>0.5</v>
+        <v>0.23255813953488369</v>
       </c>
       <c r="D1">
-        <v>0.5</v>
+        <v>0.55348837209302326</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>0.5</v>
+        <v>0.76744186046511631</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>0.5</v>
+        <v>0.23255813953488369</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>0.5</v>
+        <v>0.76744186046511631</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>0.5</v>
+        <v>0.76744186046511631</v>
       </c>
     </row>
   </sheetData>
@@ -428,7 +428,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D83B3EF1-FB1F-4217-9ED8-793CC737BA02}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{516640CE-4723-407C-99E5-30DDF7328771}">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -439,30 +439,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>0.5</v>
+        <v>0.76744186046511631</v>
       </c>
       <c r="D1">
-        <v>0.5</v>
+        <v>0.76744186046511631</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>0.5</v>
+        <v>0.76744186046511631</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>0.5</v>
+        <v>0.76744186046511631</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>0.5</v>
+        <v>0.76744186046511631</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>0.5</v>
+        <v>0.76744186046511631</v>
       </c>
     </row>
   </sheetData>
@@ -471,7 +471,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{085A71D1-7062-46E2-8348-A10CDD2571D7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06850466-7454-4BE1-B556-537D9951369B}">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -482,30 +482,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>0.5</v>
+        <v>0.76744186046511631</v>
       </c>
       <c r="D1">
-        <v>0.5</v>
+        <v>0.76744186046511631</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>0.5</v>
+        <v>0.76744186046511631</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>0.5</v>
+        <v>0.76744186046511631</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>0.5</v>
+        <v>0.76744186046511631</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>0.5</v>
+        <v>0.76744186046511631</v>
       </c>
     </row>
   </sheetData>

</xml_diff>